<commit_message>
added dummy inventory data and mapping to the page
</commit_message>
<xml_diff>
--- a/server/resources/Inventory.xlsx
+++ b/server/resources/Inventory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelevy/code/nextjs-code-challenge/server/resources/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -97,12 +97,16 @@
   </si>
   <si>
     <t>Sour Patch Kids</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -456,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFEBE3DE-3640-9646-9439-E7C7FF488907}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
@@ -464,11 +468,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.1640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="20.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -723,6 +727,16 @@
         <v>520745</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>